<commit_message>
actualizacion para presentar a domingo
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -19,14 +19,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="21">
   <si>
     <t>Method</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>bsif</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>w</t>
@@ -41,10 +40,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>accuracy</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>patches</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -53,10 +48,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>yes</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>handout 0.9</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -86,6 +77,30 @@
   </si>
   <si>
     <t>left</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>desc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gray</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>accuracy (%)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10x32</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bsif</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -460,21 +475,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="3.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -483,7 +498,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -495,27 +510,27 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J1" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>15</v>
@@ -524,30 +539,30 @@
         <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G2">
         <v>8.49</v>
       </c>
       <c r="H2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J2">
-        <v>0.70669999999999999</v>
+        <v>70.760000000000005</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <v>15</v>
@@ -556,30 +571,30 @@
         <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G3">
         <v>8.49</v>
       </c>
       <c r="H3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" t="s">
         <v>14</v>
       </c>
-      <c r="I3" t="s">
-        <v>16</v>
-      </c>
       <c r="J3">
-        <v>0.70669999999999999</v>
+        <v>70.760000000000005</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C4">
         <v>5</v>
@@ -588,22 +603,150 @@
         <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G4">
         <v>8.49</v>
       </c>
       <c r="H4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" t="s">
         <v>14</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4">
+        <v>70.760000000000005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
         <v>16</v>
       </c>
-      <c r="J4">
-        <v>0.70669999999999999</v>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5">
+        <v>5.16</v>
+      </c>
+      <c r="H5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5">
+        <v>60.67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6">
+        <v>5.58</v>
+      </c>
+      <c r="H6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7">
+        <v>15</v>
+      </c>
+      <c r="D7">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7">
+        <v>8.94</v>
+      </c>
+      <c r="H7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8">
+        <v>8.94</v>
+      </c>
+      <c r="H8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
intento de push antes de irme a Chile
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -19,7 +19,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="71">
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
   <si>
     <t>Method</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -52,10 +60,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>tt</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>voting</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -96,18 +100,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>knn mode=1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>knn mode=10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>knn mode=10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>handout .8.1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -141,6 +133,171 @@
   </si>
   <si>
     <t>left</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>simple_test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>residual_test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bsif</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>handout .8.1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>min R</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>left</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>att (s)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bisf*</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10x32</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>knn mode, 10</t>
+  </si>
+  <si>
+    <t>knn mode, 1</t>
+  </si>
+  <si>
+    <t>knn mode ,  1</t>
+  </si>
+  <si>
+    <t>Sensibilidad</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cross val</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bsifN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src_test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>splitSrc_test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>simple2_test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>row 1:11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>row 2:11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prepros</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>prepros</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>params</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>decorrstretch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>none</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sharpen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[22]-[55]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Seleccion de caracteristicas</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>File</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>desc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>w</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bits</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>parametros</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>eye</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bsif-im</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1100-30-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mRMR-Juan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>left</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Selector</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -515,10 +672,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:AL14"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="AL4" sqref="AL4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -532,46 +689,80 @@
     <col min="7" max="7" width="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="3" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="5.140625" customWidth="1"/>
+    <col min="25" max="25" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="8" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="4.85546875" customWidth="1"/>
+    <col min="29" max="29" width="11.5703125" customWidth="1"/>
+    <col min="30" max="30" width="10.140625" customWidth="1"/>
+    <col min="31" max="31" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="3" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="8.5703125" customWidth="1"/>
+    <col min="37" max="37" width="3.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:38">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" t="s">
+        <v>41</v>
+      </c>
+      <c r="U1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:38">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
       </c>
       <c r="C2">
         <v>15</v>
@@ -580,30 +771,114 @@
         <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G2">
         <v>8.49</v>
       </c>
       <c r="H2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J2">
         <v>70.760000000000005</v>
       </c>
+      <c r="K2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" t="s">
+        <v>4</v>
+      </c>
+      <c r="N2" t="s">
+        <v>5</v>
+      </c>
+      <c r="O2" t="s">
+        <v>6</v>
+      </c>
+      <c r="P2" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>35</v>
+      </c>
+      <c r="R2" t="s">
+        <v>10</v>
+      </c>
+      <c r="S2" t="s">
+        <v>12</v>
+      </c>
+      <c r="T2" t="s">
+        <v>17</v>
+      </c>
+      <c r="U2" t="s">
+        <v>2</v>
+      </c>
+      <c r="V2" t="s">
+        <v>14</v>
+      </c>
+      <c r="W2" t="s">
+        <v>4</v>
+      </c>
+      <c r="X2" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>70</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:38">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C3">
         <v>15</v>
@@ -612,30 +887,114 @@
         <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G3">
         <v>8.49</v>
       </c>
       <c r="H3" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="I3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J3">
         <v>70.760000000000005</v>
       </c>
+      <c r="K3" t="s">
+        <v>48</v>
+      </c>
+      <c r="L3" t="s">
+        <v>46</v>
+      </c>
+      <c r="M3">
+        <v>9</v>
+      </c>
+      <c r="N3">
+        <v>12</v>
+      </c>
+      <c r="O3" t="s">
+        <v>42</v>
+      </c>
+      <c r="P3" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>44</v>
+      </c>
+      <c r="R3" t="s">
+        <v>45</v>
+      </c>
+      <c r="S3" t="s">
+        <v>13</v>
+      </c>
+      <c r="T3">
+        <v>91.93</v>
+      </c>
+      <c r="U3" t="s">
+        <v>48</v>
+      </c>
+      <c r="V3" t="s">
+        <v>46</v>
+      </c>
+      <c r="W3">
+        <v>9</v>
+      </c>
+      <c r="X3">
+        <v>12</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC3">
+        <v>91.07</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>66</v>
+      </c>
+      <c r="AF3">
+        <v>11</v>
+      </c>
+      <c r="AG3">
+        <v>8</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AL3">
+        <v>95</v>
+      </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:38">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C4">
         <v>5</v>
@@ -644,94 +1003,238 @@
         <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G4">
         <v>8.49</v>
       </c>
       <c r="H4" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="I4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J4">
         <v>70.760000000000005</v>
       </c>
+      <c r="K4" t="s">
+        <v>47</v>
+      </c>
+      <c r="L4" t="s">
+        <v>46</v>
+      </c>
+      <c r="M4">
+        <v>17</v>
+      </c>
+      <c r="N4">
+        <v>12</v>
+      </c>
+      <c r="O4" t="s">
+        <v>42</v>
+      </c>
+      <c r="P4" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>44</v>
+      </c>
+      <c r="R4" t="s">
+        <v>45</v>
+      </c>
+      <c r="S4" t="s">
+        <v>13</v>
+      </c>
+      <c r="T4">
+        <v>91.13</v>
+      </c>
+      <c r="U4" t="s">
+        <v>48</v>
+      </c>
+      <c r="V4" t="s">
+        <v>46</v>
+      </c>
+      <c r="W4">
+        <v>9</v>
+      </c>
+      <c r="X4">
+        <v>12</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC4">
+        <v>91.6</v>
+      </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:38">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G5">
         <v>5.16</v>
       </c>
       <c r="H5" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="I5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J5">
         <v>60.67</v>
       </c>
+      <c r="K5" t="s">
+        <v>47</v>
+      </c>
+      <c r="L5" t="s">
+        <v>46</v>
+      </c>
+      <c r="M5">
+        <v>17</v>
+      </c>
+      <c r="N5">
+        <v>12</v>
+      </c>
+      <c r="O5" t="s">
+        <v>42</v>
+      </c>
+      <c r="P5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>44</v>
+      </c>
+      <c r="R5" t="s">
+        <v>45</v>
+      </c>
+      <c r="S5" t="s">
+        <v>13</v>
+      </c>
+      <c r="T5">
+        <v>91.73</v>
+      </c>
+      <c r="U5" t="s">
+        <v>48</v>
+      </c>
+      <c r="V5" t="s">
+        <v>46</v>
+      </c>
+      <c r="W5">
+        <v>9</v>
+      </c>
+      <c r="X5">
+        <v>12</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC5">
+        <v>90.4</v>
+      </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:38">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G6">
         <v>5.58</v>
       </c>
       <c r="H6" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="I6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J6">
         <v>64</v>
       </c>
+      <c r="K6" t="s">
+        <v>48</v>
+      </c>
+      <c r="L6" t="s">
+        <v>46</v>
+      </c>
+      <c r="M6">
+        <v>9</v>
+      </c>
+      <c r="N6">
+        <v>12</v>
+      </c>
+      <c r="O6" t="s">
+        <v>42</v>
+      </c>
+      <c r="P6" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>44</v>
+      </c>
+      <c r="R6" t="s">
+        <v>45</v>
+      </c>
+      <c r="S6" t="s">
+        <v>13</v>
+      </c>
+      <c r="T6">
+        <v>92</v>
+      </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:38">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C7">
         <v>15</v>
@@ -740,30 +1243,30 @@
         <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G7">
         <v>8.94</v>
       </c>
       <c r="H7" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="I7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J7">
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:38">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C8">
         <v>5</v>
@@ -772,30 +1275,30 @@
         <v>11</v>
       </c>
       <c r="E8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G8">
         <v>8.94</v>
       </c>
       <c r="H8" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="I8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J8">
         <v>87.33</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:38">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C9">
         <v>5</v>
@@ -804,30 +1307,30 @@
         <v>11</v>
       </c>
       <c r="E9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G9">
         <v>7.58</v>
       </c>
       <c r="H9" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="I9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J9">
         <v>83.33</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:38">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C10">
         <v>5</v>
@@ -836,54 +1339,150 @@
         <v>11</v>
       </c>
       <c r="E10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G10">
         <v>7.58</v>
       </c>
       <c r="H10" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="I10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J10">
         <v>82.5</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:38">
       <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
         <v>24</v>
       </c>
-      <c r="B11" t="s">
+      <c r="D11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" t="s">
         <v>25</v>
       </c>
-      <c r="C11" t="s">
+      <c r="G11" t="s">
         <v>26</v>
       </c>
-      <c r="D11" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" t="s">
-        <v>22</v>
-      </c>
-      <c r="F11" t="s">
+      <c r="H11" t="s">
         <v>27</v>
       </c>
-      <c r="G11" t="s">
+      <c r="I11" t="s">
         <v>28</v>
-      </c>
-      <c r="H11" t="s">
-        <v>29</v>
-      </c>
-      <c r="I11" t="s">
-        <v>30</v>
       </c>
       <c r="J11">
         <v>63.33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:38">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12">
+        <v>5</v>
+      </c>
+      <c r="D12">
+        <v>11</v>
+      </c>
+      <c r="E12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" t="s">
+        <v>37</v>
+      </c>
+      <c r="G12">
+        <v>125.22</v>
+      </c>
+      <c r="H12" t="s">
+        <v>33</v>
+      </c>
+      <c r="I12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J12">
+        <v>86.67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:38">
+      <c r="A13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13">
+        <v>5</v>
+      </c>
+      <c r="D13">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" t="s">
+        <v>37</v>
+      </c>
+      <c r="G13">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H13" t="s">
+        <v>40</v>
+      </c>
+      <c r="I13" t="s">
+        <v>34</v>
+      </c>
+      <c r="J13">
+        <v>68.33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:38">
+      <c r="A14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <v>11</v>
+      </c>
+      <c r="E14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" t="s">
+        <v>37</v>
+      </c>
+      <c r="G14">
+        <v>35</v>
+      </c>
+      <c r="H14" t="s">
+        <v>40</v>
+      </c>
+      <c r="I14" t="s">
+        <v>34</v>
+      </c>
+      <c r="J14">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>